<commit_message>
Last Update 11-01-2019 14:57:29.95
</commit_message>
<xml_diff>
--- a/Hack-List.xlsx
+++ b/Hack-List.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="151">
   <si>
     <t>KGiSL Institute of Technology</t>
   </si>
@@ -451,6 +451,33 @@
   </si>
   <si>
     <t>antonyraj0098@gmail.com</t>
+  </si>
+  <si>
+    <t>iDroid</t>
+  </si>
+  <si>
+    <t>Gowri.P</t>
+  </si>
+  <si>
+    <t>gowripasupathiraja@gmail.com</t>
+  </si>
+  <si>
+    <t>Divya.S</t>
+  </si>
+  <si>
+    <t>divyasakthi0209@gmail.com</t>
+  </si>
+  <si>
+    <t>Pragatheeswari.M</t>
+  </si>
+  <si>
+    <t>pragatheeswari333@gmail.com</t>
+  </si>
+  <si>
+    <t>Sribhavadharani S</t>
+  </si>
+  <si>
+    <t>bhavasuresh279@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -516,7 +543,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -541,6 +568,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1403,6 +1431,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A6:A9"/>
     <mergeCell ref="A32:A37"/>
     <mergeCell ref="A38:A40"/>
     <mergeCell ref="A41:A42"/>
@@ -1410,12 +1444,6 @@
     <mergeCell ref="A16:A20"/>
     <mergeCell ref="A21:A26"/>
     <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A6:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1427,10 +1455,10 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C17:C19"/>
+      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1439,11 +1467,11 @@
     <col min="2" max="2" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="6" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1540,7 +1568,9 @@
       <c r="A6" s="8">
         <v>1</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="8" t="s">
+        <v>142</v>
+      </c>
       <c r="C6" s="8" t="s">
         <v>72</v>
       </c>
@@ -1559,7 +1589,7 @@
       <c r="H6" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="10">
         <v>7708808113</v>
       </c>
     </row>
@@ -1582,7 +1612,7 @@
       <c r="H7" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="10">
         <v>8124235955</v>
       </c>
     </row>
@@ -1605,7 +1635,7 @@
       <c r="H8" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="10">
         <v>8940788301</v>
       </c>
     </row>
@@ -1628,7 +1658,7 @@
       <c r="H9" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="10">
         <v>7667733055</v>
       </c>
     </row>
@@ -1651,7 +1681,7 @@
       <c r="H10" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="10">
         <v>9789131377</v>
       </c>
     </row>
@@ -1676,7 +1706,7 @@
       <c r="H11" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="10">
         <v>9600469189</v>
       </c>
     </row>
@@ -1699,7 +1729,7 @@
       <c r="H12" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="10">
         <v>7539995743</v>
       </c>
     </row>
@@ -1722,7 +1752,7 @@
       <c r="H13" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="10">
         <v>9385665188</v>
       </c>
     </row>
@@ -1745,7 +1775,7 @@
       <c r="H14" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14" s="10">
         <v>8098420217</v>
       </c>
     </row>
@@ -1768,7 +1798,7 @@
       <c r="H15" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="10">
         <v>8525887283</v>
       </c>
     </row>
@@ -1791,7 +1821,7 @@
       <c r="H16" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16" s="10">
         <v>8946018655</v>
       </c>
     </row>
@@ -1816,7 +1846,7 @@
       <c r="H17" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17" s="10">
         <v>9047621449</v>
       </c>
     </row>
@@ -1839,7 +1869,7 @@
       <c r="H18" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18" s="10">
         <v>9486077810</v>
       </c>
     </row>
@@ -1862,7 +1892,7 @@
       <c r="H19" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I19" s="10">
         <v>7598297335</v>
       </c>
     </row>
@@ -1873,7 +1903,7 @@
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="3" t="s">
-        <v>27</v>
+        <v>149</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>9</v>
@@ -1883,6 +1913,12 @@
       </c>
       <c r="G20" s="3" t="s">
         <v>62</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="I20" s="10">
+        <v>9384751315</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1904,7 +1940,7 @@
       <c r="H21" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="I21" s="1">
+      <c r="I21" s="10">
         <v>8248658700</v>
       </c>
     </row>
@@ -1927,7 +1963,7 @@
       <c r="H22" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I22" s="10">
         <v>8610380205</v>
       </c>
     </row>
@@ -1936,7 +1972,7 @@
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="3" t="s">
-        <v>30</v>
+        <v>143</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>9</v>
@@ -1946,6 +1982,12 @@
       </c>
       <c r="G23" s="3" t="s">
         <v>62</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="I23" s="10">
+        <v>9751508828</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1953,7 +1995,7 @@
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="3" t="s">
-        <v>31</v>
+        <v>145</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>9</v>
@@ -1963,6 +2005,12 @@
       </c>
       <c r="G24" s="3" t="s">
         <v>62</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="I24" s="10">
+        <v>8903069135</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1970,7 +2018,7 @@
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="3" t="s">
-        <v>32</v>
+        <v>147</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>9</v>
@@ -1980,6 +2028,12 @@
       </c>
       <c r="G25" s="3" t="s">
         <v>62</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="I25" s="10">
+        <v>8940924877</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -2007,7 +2061,7 @@
       <c r="H26" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="I26" s="1">
+      <c r="I26" s="10">
         <v>9629595720</v>
       </c>
     </row>
@@ -2030,7 +2084,7 @@
       <c r="H27" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="I27" s="1">
+      <c r="I27" s="10">
         <v>7867996603</v>
       </c>
     </row>
@@ -2053,7 +2107,7 @@
       <c r="H28" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="I28" s="1">
+      <c r="I28" s="10">
         <v>9715418663</v>
       </c>
     </row>
@@ -2076,7 +2130,7 @@
       <c r="H29" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="I29" s="1">
+      <c r="I29" s="10">
         <v>6383817797</v>
       </c>
     </row>
@@ -2099,7 +2153,7 @@
       <c r="H30" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="I30" s="1">
+      <c r="I30" s="10">
         <v>9095031690</v>
       </c>
     </row>
@@ -2122,7 +2176,7 @@
       <c r="H31" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="I31" s="1">
+      <c r="I31" s="10">
         <v>9629163886</v>
       </c>
     </row>
@@ -2147,7 +2201,7 @@
       <c r="H32" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="I32" s="1">
+      <c r="I32" s="10">
         <v>9786498218</v>
       </c>
     </row>
@@ -2170,7 +2224,7 @@
       <c r="H33" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="I33" s="1">
+      <c r="I33" s="10">
         <v>9080574358</v>
       </c>
     </row>
@@ -2193,7 +2247,7 @@
       <c r="H34" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="I34" s="1">
+      <c r="I34" s="10">
         <v>9500760509</v>
       </c>
     </row>
@@ -2216,7 +2270,7 @@
       <c r="H35" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="I35" s="1">
+      <c r="I35" s="10">
         <v>8637435224</v>
       </c>
     </row>
@@ -2245,7 +2299,7 @@
       <c r="H36" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="I36" s="1">
+      <c r="I36" s="10">
         <v>8012246597</v>
       </c>
     </row>
@@ -2268,7 +2322,7 @@
       <c r="H37" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="I37" s="1">
+      <c r="I37" s="10">
         <v>9842749133</v>
       </c>
     </row>
@@ -2291,7 +2345,7 @@
       <c r="H38" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="I38" s="1">
+      <c r="I38" s="10">
         <v>8220402169</v>
       </c>
     </row>
@@ -2314,7 +2368,7 @@
       <c r="H39" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="I39" s="1">
+      <c r="I39" s="10">
         <v>8870566415</v>
       </c>
     </row>
@@ -2343,7 +2397,7 @@
       <c r="H40" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="I40" s="1">
+      <c r="I40" s="10">
         <v>8248972260</v>
       </c>
     </row>
@@ -2366,7 +2420,7 @@
       <c r="H41" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="I41" s="1">
+      <c r="I41" s="10">
         <v>9443889820</v>
       </c>
     </row>
@@ -2389,7 +2443,7 @@
       <c r="H42" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="I42" s="1">
+      <c r="I42" s="10">
         <v>8668161264</v>
       </c>
     </row>
@@ -2418,7 +2472,7 @@
       <c r="H43" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="I43" s="1">
+      <c r="I43" s="10">
         <v>9789612615</v>
       </c>
     </row>
@@ -2441,7 +2495,7 @@
       <c r="H44" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="I44" s="1">
+      <c r="I44" s="10">
         <v>9943922121</v>
       </c>
     </row>
@@ -2464,7 +2518,7 @@
       <c r="H45" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="I45" s="1">
+      <c r="I45" s="10">
         <v>8608201560</v>
       </c>
     </row>
@@ -2493,7 +2547,7 @@
       <c r="H46" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="I46" s="1">
+      <c r="I46" s="10">
         <v>9003987711</v>
       </c>
     </row>
@@ -2516,7 +2570,7 @@
       <c r="H47" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="I47" s="1">
+      <c r="I47" s="10">
         <v>8190027466</v>
       </c>
     </row>
@@ -2541,7 +2595,7 @@
       <c r="H48" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="I48" s="1">
+      <c r="I48" s="10">
         <v>7904048564</v>
       </c>
     </row>
@@ -2564,23 +2618,39 @@
       <c r="H49" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="I49" s="1">
+      <c r="I49" s="10">
         <v>9790678240</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="C20:C25"/>
+    <mergeCell ref="C26:C31"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="B6:B10"/>
     <mergeCell ref="A11:A16"/>
     <mergeCell ref="C6:C10"/>
     <mergeCell ref="C11:C16"/>
     <mergeCell ref="A48:A49"/>
     <mergeCell ref="B48:B49"/>
     <mergeCell ref="C48:C49"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A6:A10"/>
     <mergeCell ref="B32:B35"/>
     <mergeCell ref="B36:B39"/>
     <mergeCell ref="B40:B42"/>
@@ -2589,24 +2659,8 @@
     <mergeCell ref="A26:A31"/>
     <mergeCell ref="A32:A35"/>
     <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B6:B10"/>
     <mergeCell ref="B11:B16"/>
     <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B20:B25"/>
-    <mergeCell ref="B26:B31"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="C20:C25"/>
-    <mergeCell ref="C26:C31"/>
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A40:A42"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H43" r:id="rId1"/>
@@ -2649,8 +2703,12 @@
     <hyperlink ref="H21" r:id="rId38"/>
     <hyperlink ref="H48" r:id="rId39"/>
     <hyperlink ref="H49" r:id="rId40"/>
+    <hyperlink ref="H23" r:id="rId41"/>
+    <hyperlink ref="H24" r:id="rId42"/>
+    <hyperlink ref="H25" r:id="rId43"/>
+    <hyperlink ref="H20" r:id="rId44"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId41"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId45"/>
 </worksheet>
 </file>
</xml_diff>